<commit_message>
Refactor: Move Notion secrets to .env file and add env example
</commit_message>
<xml_diff>
--- a/favorite.xlsx
+++ b/favorite.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -451,10 +451,10 @@
         <v>2026-01-19</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H2" t="str">
-        <v>无法获取有效的视频下载地址 (可能是Blob加密流)</v>
+        <v/>
       </c>
       <c r="I2" t="str">
         <v/>
@@ -866,9 +866,183 @@
         <v/>
       </c>
     </row>
+    <row r="17">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="str">
+        <v>扣子2.0全新升级！快来看看我开发的网页应用吧</v>
+      </c>
+      <c r="C17" t="str">
+        <v>视频</v>
+      </c>
+      <c r="D17" t="str">
+        <v>#扣子编程</v>
+      </c>
+      <c r="E17" t="str">
+        <v>https://www.toutiao.com/video/7597347992571478528/</v>
+      </c>
+      <c r="F17" t="str">
+        <v>2026-01-20</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17" t="str">
+        <v>videos\2026-01-20\16.mp4</v>
+      </c>
+      <c r="I17" t="str">
+        <v>已提取</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Claude Cowork（实测）：这新功能太上头了，我可能要玩上瘾！</v>
+      </c>
+      <c r="C18" t="str">
+        <v>视频</v>
+      </c>
+      <c r="D18" t="str">
+        <v>#ClaudeCowork</v>
+      </c>
+      <c r="E18" t="str">
+        <v>https://www.toutiao.com/video/7595140659170771491/</v>
+      </c>
+      <c r="F18" t="str">
+        <v>2026-01-20</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18" t="str">
+        <v>videos\2026-01-20\17.mp4</v>
+      </c>
+      <c r="I18" t="str">
+        <v>已提取</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="str">
+        <v>用上这个Skill，你的Claude Code/Codex 将会比别人快5倍 -- 用分布式思维驯服AI任务编排</v>
+      </c>
+      <c r="C19" t="str">
+        <v>文章</v>
+      </c>
+      <c r="D19" t="str">
+        <v>无分类</v>
+      </c>
+      <c r="E19" t="str">
+        <v>https://www.toutiao.com/article/7594654759382991398/</v>
+      </c>
+      <c r="F19" t="str">
+        <v>2026-01-20</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" t="str">
+        <v>articles\2026-01-20\18.txt</v>
+      </c>
+      <c r="I19" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="str">
+        <v>为什么Agent总是Demo猛如龙实战一条虫？</v>
+      </c>
+      <c r="C20" t="str">
+        <v>文章</v>
+      </c>
+      <c r="D20" t="str">
+        <v>无分类</v>
+      </c>
+      <c r="E20" t="str">
+        <v>https://www.toutiao.com/article/7586626602591732262/</v>
+      </c>
+      <c r="F20" t="str">
+        <v>2026-01-20</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" t="str">
+        <v>articles\2026-01-20\19.txt</v>
+      </c>
+      <c r="I20" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="str">
+        <v>手把手教你用上开源版Claude Code，人人都可以体验编程Agent的魅力了。</v>
+      </c>
+      <c r="C21" t="str">
+        <v>文章</v>
+      </c>
+      <c r="D21" t="str">
+        <v>无分类</v>
+      </c>
+      <c r="E21" t="str">
+        <v>https://www.toutiao.com/article/7594454191276294719/</v>
+      </c>
+      <c r="F21" t="str">
+        <v>2026-01-20</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21" t="str">
+        <v>articles\2026-01-20\20.txt</v>
+      </c>
+      <c r="I21" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="str">
+        <v>结合 Cluade Code，我为项目设计了一个 SKILL，AI 输出代码可用率达到了 99%，谈谈真实的使用感受</v>
+      </c>
+      <c r="C22" t="str">
+        <v>文章</v>
+      </c>
+      <c r="D22" t="str">
+        <v>无分类</v>
+      </c>
+      <c r="E22" t="str">
+        <v>https://www.toutiao.com/article/7596202303636439552/</v>
+      </c>
+      <c r="F22" t="str">
+        <v>2026-01-20</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" t="str">
+        <v>articles\2026-01-20\21.txt</v>
+      </c>
+      <c r="I22" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I16"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I22"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>